<commit_message>
Feat: add Stop Exception
</commit_message>
<xml_diff>
--- a/income_report/2563/wiput888.me หวยไทย 1 พฤศจิกายน 2563 (Income).xlsx
+++ b/income_report/2563/wiput888.me หวยไทย 1 พฤศจิกายน 2563 (Income).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natthawut\Desktop\rpa-final-project\income_report\2563\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poksu\Documents\Work\KMITL\RPA\After_midterm\RPA_Final_Project\income_report\2563\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEA2415-211D-46EF-A288-FDDE4AE6146A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB348EDB-29FD-4D6D-ACEA-1D23EDEEF8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="10584" windowHeight="8016" xr2:uid="{EB12BA50-82DD-42CA-B5A2-8D19EDB5FA96}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{BD0DEB7E-EA7E-45CE-9BE3-012A7FD24FFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Income Report" sheetId="2" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,12 +403,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE20FD30-1699-4D9F-B6FB-2C5D4F02A223}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF228CB-0209-44E3-BA81-2CEAA20C1CC4}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -456,7 +459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A372BBE6-5CA1-419F-8DAA-0B73A168C4C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3442A4-B7ED-4CE2-B0DD-63D758EB654B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>